<commit_message>
configured project for selenium support in local for chrome driver version 87
</commit_message>
<xml_diff>
--- a/requirements/estimation.xlsx
+++ b/requirements/estimation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\upwork\personal_projects\WebScraping\stock-notifier-temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\upwork\personal_projects\WebScraping\stock-notifier\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AED32FD-6590-475E-8623-1095227494FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C738259E-FC32-4453-B29E-CEF5810C98D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,10 +446,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -459,8 +459,12 @@
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">

</xml_diff>

<commit_message>
added some support for ebuyer retailer site [WIP]
</commit_message>
<xml_diff>
--- a/requirements/estimation.xlsx
+++ b/requirements/estimation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\upwork\personal_projects\WebScraping\stock-notifier\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C738259E-FC32-4453-B29E-CEF5810C98D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F99F77B-543C-4A61-AB16-165910A7AF77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,8 +473,12 @@
       <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">

</xml_diff>

<commit_message>
added debugger for python file
</commit_message>
<xml_diff>
--- a/requirements/estimation.xlsx
+++ b/requirements/estimation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\upwork\personal_projects\WebScraping\stock-notifier\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F99F77B-543C-4A61-AB16-165910A7AF77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E515B6-AB00-4ED6-A3AD-F104AAF09FF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>% complete</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Documentation with all the steps</t>
+  </si>
+  <si>
+    <t>set python selenium debugger</t>
+  </si>
+  <si>
+    <t>Final total</t>
   </si>
 </sst>
 </file>
@@ -113,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -123,6 +129,9 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -404,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,7 +573,10 @@
         <f>SUM(B3:B12)</f>
         <v>22.5</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2">
+        <f>SUM(C3:C12)</f>
+        <v>4</v>
+      </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -580,10 +592,18 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
@@ -591,6 +611,19 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4">
+        <f>SUM(B14,B17:B18)</f>
+        <v>23.5</v>
+      </c>
+      <c r="C20" s="4">
+        <f>SUM(C14, C17:C18)</f>
+        <v>4.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>